<commit_message>
workin on the report
</commit_message>
<xml_diff>
--- a/Calculations/PT415 Cooling Power.xlsx
+++ b/Calculations/PT415 Cooling Power.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freyja\Documents\Cryorefrigerator\Calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF799F9-2304-4389-8C4B-246C9E5DE9D2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A0B99C-5DA3-40C1-AD7D-296856D7F60D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12165" activeTab="1" xr2:uid="{13DEEBD0-3F33-4DE5-A41C-63D5BE1F4E1A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,6 +56,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -137,9 +138,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1027,88 +1027,88 @@
             <c:numRef>
               <c:f>'Heat Capacity'!$G$5:$G$31</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>5.87664798E-2</c:v>
+                  <c:v>7.7672477702864104E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.198336869</c:v>
+                  <c:v>0.26214461224716601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47013183800000002</c:v>
+                  <c:v>0.62137982162291305</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.91822624600000002</c:v>
+                  <c:v>1.21363246410586</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.58669495</c:v>
+                  <c:v>2.0971568971919399</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5196128099999999</c:v>
+                  <c:v>3.33020741006395</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.7610545000000002</c:v>
+                  <c:v>4.9710364941328198</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3550917699999996</c:v>
+                  <c:v>7.0778761824956202</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.3457733200000002</c:v>
+                  <c:v>9.7088319631159301</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.758158099999999</c:v>
+                  <c:v>32.654839627274498</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57.763564899999999</c:v>
+                  <c:v>75.207055066786793</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>107.168164</c:v>
+                  <c:v>136.047080394651</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>168.78496000000001</c:v>
+                  <c:v>207.91337938366101</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>236.25007099999999</c:v>
+                  <c:v>282.67781760231202</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>303.97441300000003</c:v>
+                  <c:v>354.49886740052602</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>368.25538799999998</c:v>
+                  <c:v>420.22057600727902</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>427.14456899999999</c:v>
+                  <c:v>478.64819117762801</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>526.61313900000005</c:v>
+                  <c:v>574.02899299615103</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>603.49381500000004</c:v>
+                  <c:v>645.28014872583105</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>662.30664200000001</c:v>
+                  <c:v>698.50373529561705</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>707.49105899999995</c:v>
+                  <c:v>738.70080171624295</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>742.56826599999999</c:v>
+                  <c:v>769.51537064610102</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>770.14558299999999</c:v>
+                  <c:v>793.51196235367195</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>792.11191099999996</c:v>
+                  <c:v>812.48631582618498</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>809.83219199999996</c:v>
+                  <c:v>827.70491662166501</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>824.29879400000004</c:v>
+                  <c:v>840.072044893412</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>836.24049300000001</c:v>
+                  <c:v>850.24262103778904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1489,88 +1489,88 @@
             <c:numRef>
               <c:f>'Heat Capacity'!$J$5:$J$31</c:f>
               <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>4.8932999523809521E-2</c:v>
+                  <c:v>6.6282535543182197E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16514887301587303</c:v>
+                  <c:v>0.22370355745824</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.39146399523809522</c:v>
+                  <c:v>0.53026028434469896</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76457811746031745</c:v>
+                  <c:v>1.03566461641422</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3211909714285714</c:v>
+                  <c:v>1.78962824219118</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0980015714285711</c:v>
+                  <c:v>2.8418560323022501</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1316968253968254</c:v>
+                  <c:v>4.2419722210507</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4588700317460317</c:v>
+                  <c:v>6.0391296210994101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.1156965238095244</c:v>
+                  <c:v>8.2808254867312403</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.429039206349206</c:v>
+                  <c:v>27.354706165062701</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45.717572857142855</c:v>
+                  <c:v>59.245653134613598</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>79.122378095238091</c:v>
+                  <c:v>98.414566835284404</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>115.48575984126984</c:v>
+                  <c:v>138.293713704564</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>150.71703936507936</c:v>
+                  <c:v>174.87985829858701</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>182.64263968253968</c:v>
+                  <c:v>206.640912112698</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>210.51736031746032</c:v>
+                  <c:v>233.458224266381</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>234.38302380952379</c:v>
+                  <c:v>255.82294221855</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>271.75383333333332</c:v>
+                  <c:v>289.862868147298</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>298.54951746031747</c:v>
+                  <c:v>313.60667298094802</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>318.01095396825394</c:v>
+                  <c:v>330.53428642892698</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>332.41946507936507</c:v>
+                  <c:v>342.90497083596102</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>343.30545238095237</c:v>
+                  <c:v>352.16377023390697</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>351.69093968253969</c:v>
+                  <c:v>359.24599406495099</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>358.266226984127</c:v>
+                  <c:v>364.76970448254099</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>363.50562063492066</c:v>
+                  <c:v>369.15282988108203</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>367.7411952380952</c:v>
+                  <c:v>372.68446092813599</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>371.20983333333334</c:v>
+                  <c:v>375.56889526276098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1764,7 +1764,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Heat Capacity'!$D$3:$D$4</c15:sqref>
@@ -1808,7 +1808,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Heat Capacity'!$B$5:$B$31</c15:sqref>
@@ -1904,7 +1904,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Heat Capacity'!$D$5:$D$31</c15:sqref>
@@ -1999,7 +1999,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-954A-4DB6-B98D-91A4CF90B3AE}"/>
                   </c:ext>
@@ -2012,7 +2012,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Heat Capacity'!$E$3:$E$4</c15:sqref>
@@ -2056,7 +2056,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Heat Capacity'!$B$5:$B$31</c15:sqref>
@@ -2152,7 +2152,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Heat Capacity'!$E$5:$E$31</c15:sqref>
@@ -2247,7 +2247,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-954A-4DB6-B98D-91A4CF90B3AE}"/>
                   </c:ext>
@@ -2261,6 +2261,7 @@
         <c:axId val="1415700079"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="350"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3736,15 +3737,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>119061</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>471486</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>338136</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>80961</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>147638</xdr:rowOff>
+      <xdr:rowOff>128588</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4072,7 +4073,7 @@
   <dimension ref="C2:G12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4226,29 +4227,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FED56A5-2F9D-41D2-AA17-F012CDB45BFC}">
   <dimension ref="B3:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D4">
@@ -4266,7 +4267,7 @@
       <c r="I4" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -4283,14 +4284,14 @@
       <c r="F5">
         <v>0.29199999999999998</v>
       </c>
-      <c r="G5" s="1">
-        <v>5.87664798E-2</v>
+      <c r="G5">
+        <v>7.7672477702864104E-2</v>
       </c>
       <c r="I5">
         <v>9.9419999999999994E-2</v>
       </c>
-      <c r="J5" s="2">
-        <v>4.8932999523809521E-2</v>
+      <c r="J5">
+        <v>6.6282535543182197E-2</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -4306,14 +4307,14 @@
       <c r="F6">
         <v>0.60470000000000002</v>
       </c>
-      <c r="G6" s="1">
-        <v>0.198336869</v>
+      <c r="G6">
+        <v>0.26214461224716601</v>
       </c>
       <c r="I6">
         <v>0.2303</v>
       </c>
-      <c r="J6" s="2">
-        <v>0.16514887301587303</v>
+      <c r="J6">
+        <v>0.22370355745824</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -4329,14 +4330,14 @@
       <c r="F7">
         <v>1.048</v>
       </c>
-      <c r="G7" s="1">
-        <v>0.47013183800000002</v>
+      <c r="G7">
+        <v>0.62137982162291305</v>
       </c>
       <c r="I7">
         <v>0.46389999999999998</v>
       </c>
-      <c r="J7" s="2">
-        <v>0.39146399523809522</v>
+      <c r="J7">
+        <v>0.53026028434469896</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -4352,14 +4353,14 @@
       <c r="F8">
         <v>1.573</v>
       </c>
-      <c r="G8" s="1">
-        <v>0.91822624600000002</v>
+      <c r="G8">
+        <v>1.21363246410586</v>
       </c>
       <c r="I8">
         <v>0.85580000000000001</v>
       </c>
-      <c r="J8" s="2">
-        <v>0.76457811746031745</v>
+      <c r="J8">
+        <v>1.03566461641422</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -4375,14 +4376,14 @@
       <c r="F9">
         <v>2.2679999999999998</v>
       </c>
-      <c r="G9" s="1">
-        <v>1.58669495</v>
+      <c r="G9">
+        <v>2.0971568971919399</v>
       </c>
       <c r="I9">
         <v>1.47</v>
       </c>
-      <c r="J9" s="2">
-        <v>1.3211909714285714</v>
+      <c r="J9">
+        <v>1.78962824219118</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -4398,14 +4399,14 @@
       <c r="F10">
         <v>3.2349999999999999</v>
       </c>
-      <c r="G10" s="1">
-        <v>2.5196128099999999</v>
+      <c r="G10">
+        <v>3.33020741006395</v>
       </c>
       <c r="I10">
         <v>2.375</v>
       </c>
-      <c r="J10" s="2">
-        <v>2.0980015714285711</v>
+      <c r="J10">
+        <v>2.8418560323022501</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -4421,14 +4422,14 @@
       <c r="F11">
         <v>4.5810000000000004</v>
       </c>
-      <c r="G11" s="1">
-        <v>3.7610545000000002</v>
+      <c r="G11">
+        <v>4.9710364941328198</v>
       </c>
       <c r="I11">
         <v>3.64</v>
       </c>
-      <c r="J11" s="2">
-        <v>3.1316968253968254</v>
+      <c r="J11">
+        <v>4.2419722210507</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -4444,14 +4445,14 @@
       <c r="F12">
         <v>6.4160000000000004</v>
       </c>
-      <c r="G12" s="1">
-        <v>5.3550917699999996</v>
+      <c r="G12">
+        <v>7.0778761824956202</v>
       </c>
       <c r="I12">
         <v>5.327</v>
       </c>
-      <c r="J12" s="2">
-        <v>4.4588700317460317</v>
+      <c r="J12">
+        <v>6.0391296210994101</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -4467,14 +4468,14 @@
       <c r="F13">
         <v>8.8539999999999992</v>
       </c>
-      <c r="G13" s="1">
-        <v>7.3457733200000002</v>
+      <c r="G13">
+        <v>9.7088319631159301</v>
       </c>
       <c r="I13">
         <v>7.4909999999999997</v>
       </c>
-      <c r="J13" s="2">
-        <v>6.1156965238095244</v>
+      <c r="J13">
+        <v>8.2808254867312403</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -4490,14 +4491,14 @@
       <c r="F14">
         <v>33.450000000000003</v>
       </c>
-      <c r="G14" s="1">
-        <v>24.758158099999999</v>
+      <c r="G14">
+        <v>32.654839627274498</v>
       </c>
       <c r="I14">
         <v>26.4</v>
       </c>
-      <c r="J14" s="2">
-        <v>20.429039206349206</v>
+      <c r="J14">
+        <v>27.354706165062701</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
@@ -4513,14 +4514,14 @@
       <c r="F15">
         <v>81.96</v>
       </c>
-      <c r="G15" s="1">
-        <v>57.763564899999999</v>
+      <c r="G15">
+        <v>75.207055066786793</v>
       </c>
       <c r="I15">
         <v>57.63</v>
       </c>
-      <c r="J15" s="2">
-        <v>45.717572857142855</v>
+      <c r="J15">
+        <v>59.245653134613598</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -4536,14 +4537,14 @@
       <c r="F16">
         <v>148.80000000000001</v>
       </c>
-      <c r="G16" s="1">
-        <v>107.168164</v>
+      <c r="G16">
+        <v>136.047080394651</v>
       </c>
       <c r="I16">
         <v>95.84</v>
       </c>
-      <c r="J16" s="2">
-        <v>79.122378095238091</v>
+      <c r="J16">
+        <v>98.414566835284404</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -4559,14 +4560,14 @@
       <c r="F17">
         <v>223.6</v>
       </c>
-      <c r="G17" s="1">
-        <v>168.78496000000001</v>
+      <c r="G17">
+        <v>207.91337938366101</v>
       </c>
       <c r="I17">
         <v>135.19999999999999</v>
       </c>
-      <c r="J17" s="2">
-        <v>115.48575984126984</v>
+      <c r="J17">
+        <v>138.293713704564</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -4582,14 +4583,14 @@
       <c r="F18">
         <v>298.3</v>
       </c>
-      <c r="G18" s="1">
-        <v>236.25007099999999</v>
+      <c r="G18">
+        <v>282.67781760231202</v>
       </c>
       <c r="I18">
         <v>171.8</v>
       </c>
-      <c r="J18" s="2">
-        <v>150.71703936507936</v>
+      <c r="J18">
+        <v>174.87985829858701</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -4605,14 +4606,14 @@
       <c r="F19">
         <v>368.7</v>
       </c>
-      <c r="G19" s="1">
-        <v>303.97441300000003</v>
+      <c r="G19">
+        <v>354.49886740052602</v>
       </c>
       <c r="I19">
         <v>203.8</v>
       </c>
-      <c r="J19" s="2">
-        <v>182.64263968253968</v>
+      <c r="J19">
+        <v>206.640912112698</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -4628,14 +4629,14 @@
       <c r="F20">
         <v>433.3</v>
       </c>
-      <c r="G20" s="1">
-        <v>368.25538799999998</v>
+      <c r="G20">
+        <v>420.22057600727902</v>
       </c>
       <c r="I20">
         <v>230.9</v>
       </c>
-      <c r="J20" s="2">
-        <v>210.51736031746032</v>
+      <c r="J20">
+        <v>233.458224266381</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -4651,14 +4652,14 @@
       <c r="F21">
         <v>492.2</v>
       </c>
-      <c r="G21" s="1">
-        <v>427.14456899999999</v>
+      <c r="G21">
+        <v>478.64819117762801</v>
       </c>
       <c r="I21">
         <v>253.5</v>
       </c>
-      <c r="J21" s="2">
-        <v>234.38302380952379</v>
+      <c r="J21">
+        <v>255.82294221855</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -4674,14 +4675,14 @@
       <c r="F22">
         <v>594.1</v>
       </c>
-      <c r="G22" s="1">
-        <v>526.61313900000005</v>
+      <c r="G22">
+        <v>574.02899299615103</v>
       </c>
       <c r="I22">
         <v>287.60000000000002</v>
       </c>
-      <c r="J22" s="2">
-        <v>271.75383333333332</v>
+      <c r="J22">
+        <v>289.862868147298</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -4697,14 +4698,14 @@
       <c r="F23">
         <v>677.6</v>
       </c>
-      <c r="G23" s="1">
-        <v>603.49381500000004</v>
+      <c r="G23">
+        <v>645.28014872583105</v>
       </c>
       <c r="I23">
         <v>311.60000000000002</v>
       </c>
-      <c r="J23" s="2">
-        <v>298.54951746031747</v>
+      <c r="J23">
+        <v>313.60667298094802</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -4720,14 +4721,14 @@
       <c r="F24">
         <v>744.5</v>
       </c>
-      <c r="G24" s="1">
-        <v>662.30664200000001</v>
+      <c r="G24">
+        <v>698.50373529561705</v>
       </c>
       <c r="I24">
         <v>329.4</v>
       </c>
-      <c r="J24" s="2">
-        <v>318.01095396825394</v>
+      <c r="J24">
+        <v>330.53428642892698</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -4743,14 +4744,14 @@
       <c r="F25">
         <v>796.4</v>
       </c>
-      <c r="G25" s="1">
-        <v>707.49105899999995</v>
+      <c r="G25">
+        <v>738.70080171624295</v>
       </c>
       <c r="I25">
         <v>343.4</v>
       </c>
-      <c r="J25" s="2">
-        <v>332.41946507936507</v>
+      <c r="J25">
+        <v>342.90497083596102</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -4766,14 +4767,14 @@
       <c r="F26">
         <v>835.2</v>
       </c>
-      <c r="G26" s="1">
-        <v>742.56826599999999</v>
+      <c r="G26">
+        <v>769.51537064610102</v>
       </c>
       <c r="I26">
         <v>355</v>
       </c>
-      <c r="J26" s="2">
-        <v>343.30545238095237</v>
+      <c r="J26">
+        <v>352.16377023390697</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -4789,14 +4790,14 @@
       <c r="F27">
         <v>863.7</v>
       </c>
-      <c r="G27" s="1">
-        <v>770.14558299999999</v>
+      <c r="G27">
+        <v>793.51196235367195</v>
       </c>
       <c r="I27">
         <v>364.7</v>
       </c>
-      <c r="J27" s="2">
-        <v>351.69093968253969</v>
+      <c r="J27">
+        <v>359.24599406495099</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -4812,14 +4813,14 @@
       <c r="F28">
         <v>885.4</v>
       </c>
-      <c r="G28" s="1">
-        <v>792.11191099999996</v>
+      <c r="G28">
+        <v>812.48631582618498</v>
       </c>
       <c r="I28">
         <v>372.6</v>
       </c>
-      <c r="J28" s="2">
-        <v>358.266226984127</v>
+      <c r="J28">
+        <v>364.76970448254099</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -4835,14 +4836,14 @@
       <c r="F29">
         <v>904.6</v>
       </c>
-      <c r="G29" s="1">
-        <v>809.83219199999996</v>
+      <c r="G29">
+        <v>827.70491662166501</v>
       </c>
       <c r="I29">
         <v>378.6</v>
       </c>
-      <c r="J29" s="2">
-        <v>363.50562063492066</v>
+      <c r="J29">
+        <v>369.15282988108203</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -4858,14 +4859,14 @@
       <c r="F30">
         <v>925.8</v>
       </c>
-      <c r="G30" s="1">
-        <v>824.29879400000004</v>
+      <c r="G30">
+        <v>840.072044893412</v>
       </c>
       <c r="I30">
         <v>382.5</v>
       </c>
-      <c r="J30" s="2">
-        <v>367.7411952380952</v>
+      <c r="J30">
+        <v>372.68446092813599</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
@@ -4881,14 +4882,14 @@
       <c r="F31">
         <v>953.9</v>
       </c>
-      <c r="G31" s="1">
-        <v>836.24049300000001</v>
+      <c r="G31">
+        <v>850.24262103778904</v>
       </c>
       <c r="I31">
         <v>384</v>
       </c>
-      <c r="J31" s="2">
-        <v>371.20983333333334</v>
+      <c r="J31">
+        <v>375.56889526276098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>